<commit_message>
reorginized UserCrudTest, isolated problem with suite exicution
</commit_message>
<xml_diff>
--- a/LMS-CRM-Integration/excel/MOCK_DATA.xlsx
+++ b/LMS-CRM-Integration/excel/MOCK_DATA.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel - new\Desktop\Poludo Institute\Personal Github Repos 2019 onward\Sea2Sky_LMS-CRM_Integration\LMS-CRM-Integration\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE0C4C2-4F03-418E-8D89-73A2CA222E68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4B74C243-D2B1-4C6D-8A21-519C2C0DFE37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15405" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 

</xml_diff>